<commit_message>
Centralizado construtor de ExcelParser Unificado inputStream ao inves de File|InputStream Adicionado leitura de sheets pelo sheetNumber Metodo para saber quantidade de planilhas Parser e Importer agora implementam Closeable para centralizar o close do stream Alterações para usar Buffered[In|Out]putStream Testes leitura de planilhas(sheetNumber)
</commit_message>
<xml_diff>
--- a/src/test/resources/files/mock/planilha.xlsx
+++ b/src/test/resources/files/mock/planilha.xlsx
@@ -5,17 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="141" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="567" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>Cidade</t>
   </si>
@@ -154,7 +156,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -261,4 +263,236 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>41644</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>41641</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>41642</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>41643</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>41640</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.1"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>41644</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>41643</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>41642</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>41641</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>41640</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>